<commit_message>
Changed Additional-Board and Pinout
Sooo... I thought adding multiple Additional Module Boards would be bit much. Looked back at some older projects of mine and thought that using something like the uln2803 would be pretty neat (like 8 NPN Transitors, each 500mah and that in a DIL-18 Package IIRC) Which turns price really down, aswell as the size of the module. 
But using that one resultet in removing many extra pinouts, leaving with only 5 unused pins which will be broken out extra. This may change when the lcd pinout is finished. adding extra pinout for the additional board could also work out (as it occupies 8 pwm pins). I will look to copy that all into the schematic

Also missing: I2C EEPROM/Flash for settings
</commit_message>
<xml_diff>
--- a/ReST32 Pinout.xlsx
+++ b/ReST32 Pinout.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="253">
   <si>
     <t>X_DIR_PIN</t>
   </si>
@@ -582,49 +582,208 @@
     <t>USB</t>
   </si>
   <si>
+    <t>SERVO</t>
+  </si>
+  <si>
+    <t>ENDSTOP</t>
+  </si>
+  <si>
+    <t>H/T</t>
+  </si>
+  <si>
+    <t>STEPPER</t>
+  </si>
+  <si>
+    <t>PA13</t>
+  </si>
+  <si>
+    <t>JTMS-SWDIO</t>
+  </si>
+  <si>
+    <t>PA14</t>
+  </si>
+  <si>
+    <t>JTCK-SWCLK</t>
+  </si>
+  <si>
+    <t>SWD</t>
+  </si>
+  <si>
+    <t>NRST</t>
+  </si>
+  <si>
+    <t>BUTTON SWD</t>
+  </si>
+  <si>
+    <t>X-DIR</t>
+  </si>
+  <si>
+    <t>X-STEP</t>
+  </si>
+  <si>
+    <t>X-EN</t>
+  </si>
+  <si>
+    <t>Y-DIR</t>
+  </si>
+  <si>
+    <t>Y-STEP</t>
+  </si>
+  <si>
+    <t>Z-DIR</t>
+  </si>
+  <si>
+    <t>Y-EN</t>
+  </si>
+  <si>
+    <t>Z-STEP</t>
+  </si>
+  <si>
+    <t>Z-EN</t>
+  </si>
+  <si>
+    <t>E0-DIR</t>
+  </si>
+  <si>
+    <t>E0-STEP</t>
+  </si>
+  <si>
+    <t>E0-EN</t>
+  </si>
+  <si>
+    <t>E1-DIR</t>
+  </si>
+  <si>
+    <t>E1-STEP</t>
+  </si>
+  <si>
+    <t>E1-EN</t>
+  </si>
+  <si>
+    <t>PWM-BED</t>
+  </si>
+  <si>
+    <t>T0</t>
+  </si>
+  <si>
+    <t>PWM-HEAT0</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>PWM-HEAT1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>X-MIN</t>
+  </si>
+  <si>
+    <t>X-MAX</t>
+  </si>
+  <si>
+    <t>Y-MIN</t>
+  </si>
+  <si>
+    <t>Y-MAX</t>
+  </si>
+  <si>
+    <t>Z-MIN</t>
+  </si>
+  <si>
+    <t>Z-MAX</t>
+  </si>
+  <si>
+    <t>BL</t>
+  </si>
+  <si>
+    <t>EXTRA2</t>
+  </si>
+  <si>
+    <t>EXTRA1</t>
+  </si>
+  <si>
+    <t>EXTRA8</t>
+  </si>
+  <si>
+    <t>EXTRA9</t>
+  </si>
+  <si>
+    <t>EXTRA12</t>
+  </si>
+  <si>
+    <t>ADD</t>
+  </si>
+  <si>
+    <t>PWM-ADD0</t>
+  </si>
+  <si>
+    <t>PWM-ADD1</t>
+  </si>
+  <si>
+    <t>PWM-ADD2</t>
+  </si>
+  <si>
+    <t>PWM-ADD3</t>
+  </si>
+  <si>
+    <t>PWM-ADD4</t>
+  </si>
+  <si>
+    <t>PWM-ADD5</t>
+  </si>
+  <si>
+    <t>PWM-ADD6</t>
+  </si>
+  <si>
+    <t>PWM-ADD7</t>
+  </si>
+  <si>
     <t>EXTRA</t>
   </si>
   <si>
-    <t>SERVO</t>
-  </si>
-  <si>
-    <t>ENDSTOP</t>
-  </si>
-  <si>
-    <t>H/T</t>
-  </si>
-  <si>
-    <t>STEPPER</t>
-  </si>
-  <si>
-    <t>PA13</t>
-  </si>
-  <si>
-    <t>JTMS-SWDIO</t>
-  </si>
-  <si>
-    <t>PA14</t>
-  </si>
-  <si>
-    <t>JTCK-SWCLK</t>
-  </si>
-  <si>
-    <t>SWD</t>
-  </si>
-  <si>
-    <t>NRST</t>
-  </si>
-  <si>
-    <t>BUTTON SWD</t>
-  </si>
-  <si>
-    <t>UART5</t>
-  </si>
-  <si>
-    <t>4 Heater</t>
-  </si>
-  <si>
-    <t>3 Thermistor</t>
+    <t>UART</t>
+  </si>
+  <si>
+    <t>USB-DM</t>
+  </si>
+  <si>
+    <t>USB-DP</t>
+  </si>
+  <si>
+    <t>SWDIO</t>
+  </si>
+  <si>
+    <t>SWDCLK</t>
+  </si>
+  <si>
+    <t>SERVO1</t>
+  </si>
+  <si>
+    <t>SERVO2</t>
+  </si>
+  <si>
+    <t>SERVO3</t>
+  </si>
+  <si>
+    <t>SERVO4</t>
+  </si>
+  <si>
+    <t>RESET</t>
+  </si>
+  <si>
+    <t>I2C-SCL</t>
+  </si>
+  <si>
+    <t>I2C_SDA</t>
+  </si>
+  <si>
+    <t>BL-TX</t>
+  </si>
+  <si>
+    <t>BL-RX</t>
   </si>
 </sst>
 </file>
@@ -640,7 +799,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -683,6 +842,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -696,7 +867,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -704,6 +875,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1248,8 +1421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,7 +1434,7 @@
     <col min="5" max="5" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>55</v>
       </c>
@@ -1271,8 +1444,10 @@
       <c r="C1" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1283,10 +1458,13 @@
         <v>50</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1297,10 +1475,13 @@
         <v>51</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1311,10 +1492,13 @@
         <v>52</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1325,10 +1509,13 @@
         <v>53</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1339,24 +1526,30 @@
         <v>54</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>15</v>
       </c>
@@ -1367,10 +1560,13 @@
         <v>58</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>16</v>
       </c>
@@ -1381,10 +1577,13 @@
         <v>61</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>17</v>
       </c>
@@ -1395,10 +1594,13 @@
         <v>59</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>18</v>
       </c>
@@ -1409,10 +1611,13 @@
         <v>60</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>23</v>
       </c>
@@ -1423,10 +1628,13 @@
         <v>97</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>24</v>
       </c>
@@ -1437,10 +1645,13 @@
         <v>96</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>25</v>
       </c>
@@ -1451,10 +1662,13 @@
         <v>98</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>26</v>
       </c>
@@ -1465,10 +1679,13 @@
         <v>99</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>29</v>
       </c>
@@ -1479,7 +1696,10 @@
         <v>100</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1493,10 +1713,10 @@
         <v>101</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>198</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1510,10 +1730,10 @@
         <v>102</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>199</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1527,7 +1747,10 @@
         <v>103</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1541,7 +1764,10 @@
         <v>71</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1555,7 +1781,10 @@
         <v>72</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1569,7 +1798,10 @@
         <v>104</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1583,7 +1815,10 @@
         <v>105</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>188</v>
+        <v>229</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1741,173 +1976,155 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="5">
+      <c r="A35" s="7">
         <v>51</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
+        <v>52</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
+        <v>53</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
+        <v>54</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
+        <v>55</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
+        <v>56</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="8">
+        <v>57</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D41" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="E35" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="5">
-        <v>52</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D36" s="5" t="s">
+      <c r="E41" s="8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="8">
+        <v>58</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D42" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="E36" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
-        <v>53</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D37" s="5" t="s">
+      <c r="E42" s="8" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="8">
+        <v>59</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D43" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="E37" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="5">
-        <v>54</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D38" s="5" t="s">
+      <c r="E43" s="8" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="8">
+        <v>60</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D44" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="E38" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="5">
-        <v>55</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="E39" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="5">
-        <v>56</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="E40" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="5">
-        <v>57</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="E41" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="5">
-        <v>58</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="E42" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="5">
-        <v>59</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="E43" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="5">
-        <v>60</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="E44" t="s">
-        <v>186</v>
+      <c r="E44" s="8" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1921,7 +2138,10 @@
         <v>128</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>185</v>
+        <v>238</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1935,77 +2155,95 @@
         <v>129</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>185</v>
+        <v>238</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="5">
+      <c r="A47" s="4">
         <v>63</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="D47" s="5" t="s">
-        <v>185</v>
+      <c r="D47" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="5">
+      <c r="A48" s="4">
         <v>64</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D48" s="5" t="s">
-        <v>185</v>
+      <c r="D48" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="5">
+      <c r="A49" s="4">
         <v>65</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C49" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="D49" s="5" t="s">
-        <v>185</v>
+      <c r="D49" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="5">
+      <c r="A50" s="4">
         <v>66</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C50" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D50" s="5" t="s">
-        <v>185</v>
+      <c r="D50" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="5">
+      <c r="A51" s="4">
         <v>67</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C51" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D51" s="5" t="s">
-        <v>185</v>
+      <c r="D51" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2019,6 +2257,9 @@
         <v>144</v>
       </c>
       <c r="D52" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>180</v>
       </c>
     </row>
@@ -2033,6 +2274,9 @@
         <v>145</v>
       </c>
       <c r="D53" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E53" s="3" t="s">
         <v>180</v>
       </c>
     </row>
@@ -2049,6 +2293,9 @@
       <c r="D54" s="3" t="s">
         <v>184</v>
       </c>
+      <c r="E54" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
@@ -2063,19 +2310,25 @@
       <c r="D55" s="3" t="s">
         <v>184</v>
       </c>
+      <c r="E55" s="3" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>72</v>
       </c>
       <c r="B56" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>191</v>
-      </c>
       <c r="D56" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2083,13 +2336,16 @@
         <v>76</v>
       </c>
       <c r="B57" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="D57" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="D57" s="3" t="s">
-        <v>194</v>
+      <c r="E57" s="3" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2103,7 +2359,10 @@
         <v>171</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>185</v>
+        <v>238</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2117,41 +2376,44 @@
         <v>172</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>185</v>
+        <v>238</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="5">
+      <c r="A60" s="2">
         <v>80</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C60" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="D60" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="E60" t="s">
-        <v>197</v>
+      <c r="D60" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="5">
+      <c r="A61" s="2">
         <v>83</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C61" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D61" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="E61" t="s">
-        <v>197</v>
+      <c r="D61" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2165,7 +2427,10 @@
         <v>174</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2179,7 +2444,10 @@
         <v>175</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2193,7 +2461,10 @@
         <v>176</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2207,7 +2478,10 @@
         <v>177</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -2221,7 +2495,10 @@
         <v>178</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -2235,69 +2512,78 @@
         <v>161</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="5">
+      <c r="A68" s="7">
         <v>92</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C68" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="D68" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="E68" t="s">
+      <c r="D68" s="7" t="s">
         <v>181</v>
       </c>
+      <c r="E68" s="7" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="5">
+      <c r="A69" s="7">
         <v>93</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C69" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="D69" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="E69" t="s">
+      <c r="D69" s="7" t="s">
         <v>181</v>
       </c>
+      <c r="E69" s="7" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="5">
+      <c r="A70" s="4">
         <v>95</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="C70" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="D70" s="5" t="s">
-        <v>185</v>
+      <c r="D70" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="5">
+      <c r="A71" s="4">
         <v>96</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B71" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C71" s="5" t="s">
+      <c r="C71" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="D71" s="5" t="s">
-        <v>185</v>
+      <c r="D71" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2311,7 +2597,10 @@
         <v>150</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>185</v>
+        <v>238</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2325,7 +2614,10 @@
         <v>151</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed pin naming on excel table
</commit_message>
<xml_diff>
--- a/ReST32 Pinout.xlsx
+++ b/ReST32 Pinout.xlsx
@@ -705,13 +705,10 @@
     <t>EXTRA1</t>
   </si>
   <si>
-    <t>EXTRA8</t>
-  </si>
-  <si>
-    <t>EXTRA9</t>
-  </si>
-  <si>
-    <t>EXTRA12</t>
+    <t>EXTRA3</t>
+  </si>
+  <si>
+    <t>EXTRA4</t>
   </si>
   <si>
     <t>ADD</t>
@@ -784,6 +781,9 @@
   </si>
   <si>
     <t>BL-RX</t>
+  </si>
+  <si>
+    <t>EXTRA0</t>
   </si>
 </sst>
 </file>
@@ -1421,8 +1421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1543,7 +1543,7 @@
         <v>194</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>195</v>
@@ -1815,10 +1815,10 @@
         <v>105</v>
       </c>
       <c r="D23" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>229</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2073,7 +2073,7 @@
         <v>185</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -2090,7 +2090,7 @@
         <v>185</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2107,7 +2107,7 @@
         <v>185</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2124,7 +2124,7 @@
         <v>185</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2138,10 +2138,10 @@
         <v>128</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>225</v>
+        <v>252</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2155,10 +2155,10 @@
         <v>129</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2172,10 +2172,10 @@
         <v>139</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2189,10 +2189,10 @@
         <v>140</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -2206,10 +2206,10 @@
         <v>141</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2223,10 +2223,10 @@
         <v>142</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2240,10 +2240,10 @@
         <v>143</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2257,7 +2257,7 @@
         <v>144</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>180</v>
@@ -2274,7 +2274,7 @@
         <v>145</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>180</v>
@@ -2294,7 +2294,7 @@
         <v>184</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -2311,7 +2311,7 @@
         <v>184</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -2328,7 +2328,7 @@
         <v>193</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2345,7 +2345,7 @@
         <v>193</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2359,10 +2359,10 @@
         <v>171</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2376,10 +2376,10 @@
         <v>172</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2396,7 +2396,7 @@
         <v>223</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2413,7 +2413,7 @@
         <v>223</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2532,7 +2532,7 @@
         <v>181</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2549,7 +2549,7 @@
         <v>181</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -2563,10 +2563,10 @@
         <v>154</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2580,10 +2580,10 @@
         <v>155</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2597,10 +2597,10 @@
         <v>150</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added LCD 8080 Pinout
</commit_message>
<xml_diff>
--- a/ReST32 Pinout.xlsx
+++ b/ReST32 Pinout.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="271">
   <si>
     <t>X_DIR_PIN</t>
   </si>
@@ -726,18 +726,6 @@
     <t>PWM-ADD3</t>
   </si>
   <si>
-    <t>PWM-ADD4</t>
-  </si>
-  <si>
-    <t>PWM-ADD5</t>
-  </si>
-  <si>
-    <t>PWM-ADD6</t>
-  </si>
-  <si>
-    <t>PWM-ADD7</t>
-  </si>
-  <si>
     <t>EXTRA</t>
   </si>
   <si>
@@ -784,6 +772,72 @@
   </si>
   <si>
     <t>EXTRA0</t>
+  </si>
+  <si>
+    <t>E2-DIR</t>
+  </si>
+  <si>
+    <t>E2-STEP</t>
+  </si>
+  <si>
+    <t>E2-EN</t>
+  </si>
+  <si>
+    <t>EXTRA5</t>
+  </si>
+  <si>
+    <t>LCD Compatible with ADAFRUIT 2.8" 8080 Breakout</t>
+  </si>
+  <si>
+    <t>SPI-SCK</t>
+  </si>
+  <si>
+    <t>SPI-MISO</t>
+  </si>
+  <si>
+    <t>SPI-MOSI</t>
+  </si>
+  <si>
+    <t>SPI-CS2</t>
+  </si>
+  <si>
+    <t>SPI-CS1</t>
+  </si>
+  <si>
+    <t>LCD-D0</t>
+  </si>
+  <si>
+    <t>LCD-D1</t>
+  </si>
+  <si>
+    <t>LCD-D2</t>
+  </si>
+  <si>
+    <t>LCD-D3</t>
+  </si>
+  <si>
+    <t>LCD-D4</t>
+  </si>
+  <si>
+    <t>LCD-D5</t>
+  </si>
+  <si>
+    <t>LCD-D6</t>
+  </si>
+  <si>
+    <t>LCD-D7</t>
+  </si>
+  <si>
+    <t>LCD-CS</t>
+  </si>
+  <si>
+    <t>LCD-CD</t>
+  </si>
+  <si>
+    <t>LCD-WR</t>
+  </si>
+  <si>
+    <t>LCD-RD</t>
   </si>
 </sst>
 </file>
@@ -867,7 +921,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -877,6 +931,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1419,10 +1476,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,7 +1518,7 @@
         <v>188</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1478,7 +1535,7 @@
         <v>188</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1495,7 +1552,7 @@
         <v>188</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1512,7 +1569,7 @@
         <v>188</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1529,7 +1586,7 @@
         <v>188</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1543,7 +1600,7 @@
         <v>194</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>195</v>
@@ -1563,7 +1620,7 @@
         <v>188</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1580,7 +1637,7 @@
         <v>188</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1597,7 +1654,7 @@
         <v>188</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1614,7 +1671,7 @@
         <v>188</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1631,7 +1688,7 @@
         <v>188</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1648,7 +1705,7 @@
         <v>188</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1665,7 +1722,7 @@
         <v>188</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>208</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1682,7 +1739,7 @@
         <v>188</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>209</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1699,10 +1756,10 @@
         <v>188</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>30</v>
       </c>
@@ -1719,7 +1776,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>31</v>
       </c>
@@ -1736,7 +1793,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>32</v>
       </c>
@@ -1753,7 +1810,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>33</v>
       </c>
@@ -1770,7 +1827,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>34</v>
       </c>
@@ -1787,7 +1844,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>35</v>
       </c>
@@ -1804,7 +1861,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>36</v>
       </c>
@@ -1821,7 +1878,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>38</v>
       </c>
@@ -1834,8 +1891,17 @@
       <c r="D24" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>39</v>
       </c>
@@ -1848,8 +1914,11 @@
       <c r="D25" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>40</v>
       </c>
@@ -1862,8 +1931,11 @@
       <c r="D26" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>41</v>
       </c>
@@ -1876,8 +1948,11 @@
       <c r="D27" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>42</v>
       </c>
@@ -1890,8 +1965,11 @@
       <c r="D28" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43</v>
       </c>
@@ -1904,8 +1982,11 @@
       <c r="D29" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44</v>
       </c>
@@ -1918,8 +1999,11 @@
       <c r="D30" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>45</v>
       </c>
@@ -1932,8 +2016,11 @@
       <c r="D31" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>46</v>
       </c>
@@ -1945,6 +2032,9 @@
       </c>
       <c r="D32" s="1" t="s">
         <v>42</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1960,6 +2050,9 @@
       <c r="D33" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="E33" s="1" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
@@ -1974,6 +2067,9 @@
       <c r="D34" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="E34" s="1" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
@@ -1988,6 +2084,9 @@
       <c r="D35" s="7" t="s">
         <v>179</v>
       </c>
+      <c r="E35" s="7" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
@@ -2002,6 +2101,9 @@
       <c r="D36" s="7" t="s">
         <v>179</v>
       </c>
+      <c r="E36" s="7" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
@@ -2016,6 +2118,9 @@
       <c r="D37" s="7" t="s">
         <v>179</v>
       </c>
+      <c r="E37" s="7" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
@@ -2030,6 +2135,9 @@
       <c r="D38" s="7" t="s">
         <v>179</v>
       </c>
+      <c r="E38" s="7" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
@@ -2044,19 +2152,25 @@
       <c r="D39" s="7" t="s">
         <v>179</v>
       </c>
+      <c r="E39" s="7" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="7">
+      <c r="A40" s="1">
         <v>56</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D40" s="7" t="s">
-        <v>179</v>
+      <c r="D40" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2073,7 +2187,7 @@
         <v>185</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -2090,7 +2204,7 @@
         <v>185</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2107,7 +2221,7 @@
         <v>185</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2124,7 +2238,7 @@
         <v>185</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2138,10 +2252,10 @@
         <v>128</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2155,7 +2269,7 @@
         <v>129</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>225</v>
@@ -2213,37 +2327,37 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="4">
+      <c r="A50" s="5">
         <v>66</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="D50" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="E50" s="4" t="s">
+      <c r="D50" s="5" t="s">
         <v>233</v>
       </c>
+      <c r="E50" s="5" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="4">
+      <c r="A51" s="5">
         <v>67</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="D51" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>234</v>
+      <c r="D51" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2257,7 +2371,7 @@
         <v>144</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>180</v>
@@ -2274,7 +2388,7 @@
         <v>145</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>180</v>
@@ -2294,7 +2408,7 @@
         <v>184</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -2311,7 +2425,7 @@
         <v>184</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -2328,7 +2442,7 @@
         <v>193</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2345,7 +2459,7 @@
         <v>193</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2359,10 +2473,10 @@
         <v>171</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2376,10 +2490,10 @@
         <v>172</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>226</v>
+        <v>252</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2396,7 +2510,7 @@
         <v>223</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2413,7 +2527,7 @@
         <v>223</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2532,7 +2646,7 @@
         <v>181</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2549,58 +2663,58 @@
         <v>181</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="4">
+      <c r="A70" s="2">
         <v>95</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="C70" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D70" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>235</v>
+      <c r="D70" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="4">
+      <c r="A71" s="2">
         <v>96</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="C71" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="D71" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>236</v>
+      <c r="D71" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="5">
+      <c r="A72" s="2">
         <v>97</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C72" s="5" t="s">
+      <c r="C72" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D72" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>227</v>
+      <c r="D72" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2617,10 +2731,13 @@
         <v>188</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G24:J24"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Final Version of Main Controller Schematic
</commit_message>
<xml_diff>
--- a/ReST32 Pinout.xlsx
+++ b/ReST32 Pinout.xlsx
@@ -16,6 +16,7 @@
     <sheet name=" Pin Function VET6" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -765,12 +766,6 @@
     <t>I2C_SDA</t>
   </si>
   <si>
-    <t>BL-TX</t>
-  </si>
-  <si>
-    <t>BL-RX</t>
-  </si>
-  <si>
     <t>EXTRA0</t>
   </si>
   <si>
@@ -838,6 +833,12 @@
   </si>
   <si>
     <t>LCD-RD</t>
+  </si>
+  <si>
+    <t>UART5-TX</t>
+  </si>
+  <si>
+    <t>UART5-RX</t>
   </si>
 </sst>
 </file>
@@ -1478,8 +1479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C46" sqref="C45:C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1722,7 +1723,7 @@
         <v>188</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1739,7 +1740,7 @@
         <v>188</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1756,7 +1757,7 @@
         <v>188</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1892,10 +1893,10 @@
         <v>42</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
@@ -1915,7 +1916,7 @@
         <v>42</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1932,7 +1933,7 @@
         <v>42</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1949,7 +1950,7 @@
         <v>42</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1966,7 +1967,7 @@
         <v>42</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1983,7 +1984,7 @@
         <v>42</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2000,7 +2001,7 @@
         <v>42</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2017,7 +2018,7 @@
         <v>42</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2034,7 +2035,7 @@
         <v>42</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2051,7 +2052,7 @@
         <v>42</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -2068,7 +2069,7 @@
         <v>42</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -2085,7 +2086,7 @@
         <v>179</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -2102,7 +2103,7 @@
         <v>179</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -2119,7 +2120,7 @@
         <v>179</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -2136,7 +2137,7 @@
         <v>179</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2153,7 +2154,7 @@
         <v>179</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -2170,7 +2171,7 @@
         <v>42</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2255,7 +2256,7 @@
         <v>233</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2493,7 +2494,7 @@
         <v>233</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2510,7 +2511,7 @@
         <v>223</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>246</v>
+        <v>269</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2527,7 +2528,7 @@
         <v>223</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>247</v>
+        <v>270</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added PDF for Pinout
+removed images from logo
</commit_message>
<xml_diff>
--- a/ReST32 Pinout.xlsx
+++ b/ReST32 Pinout.xlsx
@@ -937,11 +937,11 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1556,10 +1556,10 @@
       <c r="C4" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>222</v>
       </c>
     </row>
@@ -1902,12 +1902,12 @@
       <c r="E24" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="G24" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
@@ -2726,13 +2726,13 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="11">
+      <c r="A73" s="10">
         <v>98</v>
       </c>
-      <c r="B73" s="11" t="s">
+      <c r="B73" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="C73" s="11" t="s">
+      <c r="C73" s="10" t="s">
         <v>151</v>
       </c>
       <c r="D73" s="2" t="s">

</xml_diff>

<commit_message>
Added BOM and changed Oscillator to Crystal
</commit_message>
<xml_diff>
--- a/ReST32 Pinout.xlsx
+++ b/ReST32 Pinout.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="274">
   <si>
     <t>X_DIR_PIN</t>
   </si>
@@ -838,6 +838,15 @@
   </si>
   <si>
     <t>UART5-RX</t>
+  </si>
+  <si>
+    <t>PC13</t>
+  </si>
+  <si>
+    <t>TAMPER-RTC</t>
+  </si>
+  <si>
+    <t>LED</t>
   </si>
 </sst>
 </file>
@@ -859,7 +868,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -914,6 +923,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -927,7 +942,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -942,6 +957,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1484,10 +1500,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J73"/>
+  <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1598,802 +1614,800 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="12">
+        <v>7</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>14</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>195</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <v>15</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>186</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>186</v>
       </c>
       <c r="E10" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>17</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>217</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>18</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>188</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>182</v>
+        <v>64</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>188</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>65</v>
+        <v>182</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>188</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>247</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>188</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>188</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>29</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>249</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
-        <v>30</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>187</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>187</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>187</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>187</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>187</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
+        <v>35</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
         <v>36</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E24" s="4" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>38</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>251</v>
-      </c>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>258</v>
-      </c>
+        <v>257</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E34" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>48</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>267</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="7">
-        <v>51</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>179</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>179</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>179</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>179</v>
       </c>
       <c r="E39" s="7" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
+        <v>55</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="E40" s="7" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
         <v>56</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>268</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="8">
-        <v>57</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>185</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>185</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D44" s="8" t="s">
         <v>185</v>
       </c>
       <c r="E44" s="8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="8">
+        <v>60</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="E45" s="8" t="s">
         <v>242</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="5">
-        <v>61</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>233</v>
       </c>
       <c r="E46" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
+        <v>62</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="E47" s="5" t="s">
         <v>225</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
-        <v>63</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>228</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>228</v>
       </c>
       <c r="E49" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <v>65</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="E50" s="4" t="s">
         <v>230</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="5">
-        <v>66</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>233</v>
       </c>
       <c r="E51" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="5">
+        <v>67</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="E52" s="5" t="s">
         <v>226</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="3">
-        <v>68</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>234</v>
@@ -2404,347 +2418,364 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>184</v>
+        <v>234</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>235</v>
+        <v>180</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>184</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>189</v>
+        <v>138</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>190</v>
+        <v>147</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>193</v>
       </c>
       <c r="E57" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
+        <v>76</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E58" s="3" t="s">
         <v>238</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="5">
-        <v>78</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>233</v>
       </c>
       <c r="E59" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="5">
+        <v>79</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="E60" s="5" t="s">
         <v>250</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="8">
-        <v>80</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="E60" s="8" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D61" s="8" t="s">
         <v>223</v>
       </c>
       <c r="E61" s="8" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="8">
+        <v>83</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="E62" s="8" t="s">
         <v>270</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="2">
-        <v>84</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>188</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>188</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>188</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>188</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>188</v>
       </c>
       <c r="E67" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>91</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E68" s="2" t="s">
         <v>207</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="7">
-        <v>92</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="E68" s="7" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="7">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D69" s="7" t="s">
         <v>181</v>
       </c>
       <c r="E69" s="7" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="7">
+        <v>93</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="E70" s="7" t="s">
         <v>245</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="2">
-        <v>95</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>188</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>188</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="10">
-        <v>98</v>
-      </c>
-      <c r="B73" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="C73" s="10" t="s">
-        <v>151</v>
+      <c r="A73" s="2">
+        <v>97</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>188</v>
       </c>
       <c r="E73" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="10">
+        <v>98</v>
+      </c>
+      <c r="B74" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C74" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E74" s="2" t="s">
         <v>196</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="G25:J25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>